<commit_message>
added Information and Process
</commit_message>
<xml_diff>
--- a/project/excel/split_pool_mod_schema.xlsx
+++ b/project/excel/split_pool_mod_schema.xlsx
@@ -10,6 +10,8 @@
     <sheet name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Database" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="MaterialEntity" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Process" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Information" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -451,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,12 +464,22 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>information_set</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>material_entity_set</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>named_thing_set</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>material_entity_set</t>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>process_set</t>
         </is>
       </c>
     </row>
@@ -510,4 +522,86 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_inputs</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_outputs</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
neon api -> YAML -> TTL
</commit_message>
<xml_diff>
--- a/project/excel/split_pool_mod_schema.xlsx
+++ b/project/excel/split_pool_mod_schema.xlsx
@@ -12,6 +12,27 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MaterialEntity" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Process" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Information" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MicDnaExtractionInSoilDnaSample" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MicDnaExtractionInSubsample" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SlsMetagenomicsPoolingInCompositeSample" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SlsSoilCoreCollectionInGeneticArchiveSample1" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SlsSoilCoreCollectionInGeneticArchiveSample2" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SlsSoilCoreCollectionInGeneticArchiveSample3" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SlsSoilCoreCollectionInGeneticArchiveSample4" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SlsSoilCoreCollectionInGeneticArchiveSample5" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SlsSoilCoreCollectionInGeneticSample" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SlsSoilCoreCollectionInSample" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SlsSoilMoistureInMoistureSample" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SlsSoilpHInPhSample" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MmsMetagenomeSequencingInProcessedSeqFileName" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SubsampleDnaExtract" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sequencing" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DnaSamplePrepSimple" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DnaSamplePrepComposite" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pooling" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GeneticSamplePrep" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MoistureSamplePrep" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PhSamplePrep" sheetId="26" state="visible" r:id="rId26"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -447,13 +468,608 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>neon_sample_class</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>neon_sample_tag</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>neon_sample_uuid</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_children</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>has_parents</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>neon_sample_class</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>neon_sample_tag</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>neon_sample_uuid</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_children</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>has_parents</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>neon_sample_class</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>neon_sample_tag</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>neon_sample_uuid</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_children</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>has_parents</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>neon_sample_class</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>neon_sample_tag</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>neon_sample_uuid</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_children</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>has_parents</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>neon_sample_class</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>neon_sample_tag</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>neon_sample_uuid</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_children</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>has_parents</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>neon_sample_class</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>neon_sample_tag</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>neon_sample_uuid</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_children</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>has_parents</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>neon_sample_class</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>neon_sample_tag</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>neon_sample_uuid</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_children</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>has_parents</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>neon_sample_class</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>neon_sample_tag</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>neon_sample_uuid</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_children</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>has_parents</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>neon_sample_class</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>neon_sample_tag</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>neon_sample_uuid</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_children</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>has_parents</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_inputs</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_outputs</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:AA1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -492,6 +1108,433 @@
           <t>process_set</t>
         </is>
       </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>mic_dna_extraction_in_soil_dna_sample_set</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>mic_dna_extraction_in_subsample_set</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>mms_metagenome_sequencing_in_processed_seq_file_name_set</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>sls_metagenomics_pooling_in_composite_sample_set</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>sls_soil_core_collection_in_genetic_archive_sample1_set</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>sls_soil_core_collection_in_genetic_archive_sample2_set</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>sls_soil_core_collection_in_genetic_archive_sample3_set</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>sls_soil_core_collection_in_genetic_archive_sample4_set</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>sls_soil_core_collection_in_genetic_archive_sample5_set</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>sls_soil_core_collection_in_genetic_sample_set</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>sls_soil_core_collection_in_sample_set</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>sls_soil_moisture_in_moisture_sample_set</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>sls_soil_ph_in_ph_sample_set</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>dna_sample_prep_composite_set</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>dna_sample_prep_simple_set</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>genetic_sample_prep_set</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>moisture_sample_prep_set</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>ph_sample_prep_set</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>pooling_set</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>sequencing_set</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>subsample_dna_extract_set</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_inputs</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_outputs</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_inputs</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_outputs</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_inputs</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_outputs</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_inputs</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_outputs</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_inputs</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_outputs</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_inputs</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_outputs</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_inputs</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_outputs</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -504,6 +1547,113 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>neon_sample_class</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>neon_sample_tag</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>neon_sample_uuid</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_children</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>has_parents</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_inputs</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_outputs</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -534,88 +1684,240 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>has_inputs</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>has_outputs</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>has_input</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>has_output</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>id</t>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>neon_sample_class</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>neon_sample_tag</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>neon_sample_uuid</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_children</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>has_parents</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>id</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
+          <t>name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>neon_sample_class</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>neon_sample_tag</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>neon_sample_uuid</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_children</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>has_parents</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>neon_sample_class</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>neon_sample_tag</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>neon_sample_uuid</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_children</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>has_parents</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>neon_sample_class</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>neon_sample_tag</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>neon_sample_uuid</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_children</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>has_parents</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
         <is>
           <t>description</t>
         </is>

</xml_diff>

<commit_message>
still having trouble with Database process slots
</commit_message>
<xml_diff>
--- a/project/excel/split_pool_mod_schema.xlsx
+++ b/project/excel/split_pool_mod_schema.xlsx
@@ -12,27 +12,41 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MaterialEntity" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Process" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Information" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MicDnaExtractionInSoilDnaSample" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MicDnaExtractionInSubsample" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SlsMetagenomicsPoolingInCompositeSample" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SlsSoilCoreCollectionInGeneticArchiveSample1" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SlsSoilCoreCollectionInGeneticArchiveSample2" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SlsSoilCoreCollectionInGeneticArchiveSample3" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SlsSoilCoreCollectionInGeneticArchiveSample4" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SlsSoilCoreCollectionInGeneticArchiveSample5" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SlsSoilCoreCollectionInGeneticSample" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SlsSoilCoreCollectionInSample" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SlsSoilMoistureInMoistureSample" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SlsSoilpHInPhSample" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MmsMetagenomeSequencingInProcessedSeqFileName" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SubsampleDnaExtract" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sequencing" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DnaSamplePrepSimple" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DnaSamplePrepComposite" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pooling" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GeneticSamplePrep" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MoistureSamplePrep" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PhSamplePrep" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NtrInternalLabInKclSample" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SlsBgcSubsamplingInBgcArchive" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SlsBgcSubsamplingInCnSample" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SlsSoilCoreCollectionInBiomass" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MicDnaExtractionInSoilDnaSample" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MicDnaExtractionInSubsample" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SlsMetagenomicsPoolingInCompositeSample" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SlsSoilCoreCollectionInGeneticArchiveSample" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SlsSoilCoreCollectionInGeneticArchiveSample1" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SlsSoilCoreCollectionInGeneticArchiveSample2" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SlsSoilCoreCollectionInGeneticArchiveSample3" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SlsSoilCoreCollectionInGeneticArchiveSample4" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SlsSoilCoreCollectionInGeneticArchiveSample5" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SlsSoilCoreCollectionInGeneticSample" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SlsSoilCoreCollectionInSample" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SlsSoilMoistureInMoistureSample" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SlsSoilpHInPhSample" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MmsMetagenomeSequencingInProcessedSeqFileName" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SubsampleDnaExtract" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sequencing" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DnaSamplePrepSimple" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DnaSamplePrepComposite" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pooling" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GeneticSamplePrep" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MoistureSamplePrep" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PhSamplePrep" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="KclSamplePrep" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BgcArchiving" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CnSamplePrep" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BiomassSamplePrep" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GeneticArchiving1" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GeneticArchiving2" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GeneticArchiving3" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GeneticArchiving4" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GeneticArchiving5" sheetId="40" state="visible" r:id="rId40"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1023,6 +1037,467 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>neon_sample_class</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>neon_sample_tag</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>neon_sample_uuid</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_children</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>has_parents</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AA1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>information_set</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>material_entity_set</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>named_thing_set</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>process_set</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>mic_dna_extraction_in_soil_dna_sample_set</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>mic_dna_extraction_in_subsample_set</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>mms_metagenome_sequencing_in_processed_seq_file_name_set</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>sls_metagenomics_pooling_in_composite_sample_set</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>sls_soil_core_collection_in_genetic_archive_sample1_set</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>sls_soil_core_collection_in_genetic_archive_sample2_set</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>sls_soil_core_collection_in_genetic_archive_sample3_set</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>sls_soil_core_collection_in_genetic_archive_sample4_set</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>sls_soil_core_collection_in_genetic_archive_sample5_set</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>sls_soil_core_collection_in_genetic_sample_set</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>sls_soil_core_collection_in_sample_set</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>sls_soil_moisture_in_moisture_sample_set</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>sls_soil_ph_in_ph_sample_set</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>dna_sample_prep_composite_set</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>dna_sample_prep_simple_set</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>genetic_sample_prep_set</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>moisture_sample_prep_set</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>ph_sample_prep_set</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>pooling_set</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>sequencing_set</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>subsample_dna_extract_set</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>neon_sample_class</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>neon_sample_tag</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>neon_sample_uuid</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_children</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>has_parents</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>neon_sample_class</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>neon_sample_tag</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>neon_sample_uuid</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_children</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>has_parents</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>neon_sample_class</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>neon_sample_tag</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>neon_sample_uuid</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_children</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>has_parents</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>neon_sample_class</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>neon_sample_tag</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>neon_sample_uuid</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_children</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>has_parents</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1063,163 +1538,298 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AA1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>information_set</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>material_entity_set</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>named_thing_set</t>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_inputs</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_outputs</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_inputs</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_outputs</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_inputs</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_outputs</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_inputs</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_outputs</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_inputs</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_outputs</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>neon_sample_class</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>neon_sample_tag</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>neon_sample_uuid</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_children</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>has_parents</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>process_set</t>
+          <t>id</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>mic_dna_extraction_in_soil_dna_sample_set</t>
+          <t>name</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>mic_dna_extraction_in_subsample_set</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>mms_metagenome_sequencing_in_processed_seq_file_name_set</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>sls_metagenomics_pooling_in_composite_sample_set</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>sls_soil_core_collection_in_genetic_archive_sample1_set</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>sls_soil_core_collection_in_genetic_archive_sample2_set</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>sls_soil_core_collection_in_genetic_archive_sample3_set</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>sls_soil_core_collection_in_genetic_archive_sample4_set</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>sls_soil_core_collection_in_genetic_archive_sample5_set</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>sls_soil_core_collection_in_genetic_sample_set</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>sls_soil_core_collection_in_sample_set</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>sls_soil_moisture_in_moisture_sample_set</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>sls_soil_ph_in_ph_sample_set</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>dna_sample_prep_composite_set</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>dna_sample_prep_simple_set</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>genetic_sample_prep_set</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>moisture_sample_prep_set</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>ph_sample_prep_set</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>pooling_set</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>sequencing_set</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>subsample_dna_extract_set</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1265,7 +1875,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1311,7 +1921,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1357,7 +1967,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1403,7 +2013,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1449,7 +2059,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1495,7 +2105,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1541,7 +2151,273 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_inputs</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_outputs</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_inputs</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_outputs</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_inputs</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_outputs</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_inputs</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_outputs</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>has_inputs</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>has_outputs</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1602,89 +2478,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>has_inputs</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>has_outputs</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1745,7 +2539,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1806,7 +2600,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1865,65 +2659,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>neon_sample_class</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>neon_sample_tag</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>neon_sample_uuid</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>has_children</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>has_parents</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>